<commit_message>
try running main.py guyss
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,6 +441,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="B12">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>